<commit_message>
find the multi mode in data set
</commit_message>
<xml_diff>
--- a/Ex_Files_Stats_Basic/Ex_Files_Stats_Basic/Exercise Files/02_03_Answers.xlsx
+++ b/Ex_Files_Stats_Basic/Ex_Files_Stats_Basic/Exercise Files/02_03_Answers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eddiedavila/Desktop/Stats WB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Statistics Foundations 1- The Basics\Ex_Files_Stats_Basic\Ex_Files_Stats_Basic\Exercise Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645F2157-B66B-2B4B-8D8C-18022E992F7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B43AE94-3700-4D1E-BBCD-7B53E821555A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2560" windowWidth="27380" windowHeight="15400" activeTab="6" xr2:uid="{02E90640-9AFF-EB41-9DBB-76A9E96308E5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="6" xr2:uid="{02E90640-9AFF-EB41-9DBB-76A9E96308E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Set" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="18">
   <si>
     <t>Data Point</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Avg of 10th &amp; 11th value</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -486,7 +489,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -501,16 +504,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1499,9 +1502,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1539,7 +1542,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1645,7 +1648,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1787,7 +1790,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1799,7 +1802,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
@@ -1811,7 +1814,7 @@
     <col min="10" max="10" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1827,7 +1830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1851,7 +1854,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1883,7 +1886,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1899,7 +1902,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1915,7 +1918,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1923,7 +1926,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1931,7 +1934,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1947,7 +1950,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1955,7 +1958,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1963,7 +1966,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -1979,7 +1982,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1996,7 +1999,7 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
@@ -2008,7 +2011,7 @@
     <col min="10" max="10" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2024,7 +2027,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2051,7 +2054,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2069,7 +2072,7 @@
       </c>
       <c r="J4" s="39"/>
     </row>
-    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2088,7 +2091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2107,7 +2110,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2135,7 +2138,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2143,7 +2146,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2151,7 +2154,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2180,7 +2183,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2194,7 +2197,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="31"/>
     </row>
-    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2216,7 +2219,7 @@
       <c r="I13" s="30"/>
       <c r="J13" s="31"/>
     </row>
-    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2230,7 +2233,7 @@
       <c r="I14" s="30"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2252,7 +2255,7 @@
       <c r="I15" s="33"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2260,7 +2263,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2268,7 +2271,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2276,7 +2279,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2284,7 +2287,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2292,7 +2295,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -2300,7 +2303,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2317,7 +2320,7 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
@@ -2329,7 +2332,7 @@
     <col min="10" max="10" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2337,7 +2340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2345,7 +2348,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2372,7 +2375,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2390,7 +2393,7 @@
       </c>
       <c r="J4" s="39"/>
     </row>
-    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2409,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2428,7 +2431,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2448,7 +2451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2456,7 +2459,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2501,7 +2504,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2517,7 +2520,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2539,7 +2542,7 @@
       <c r="I13" s="30"/>
       <c r="J13" s="31"/>
     </row>
-    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2553,7 +2556,7 @@
       <c r="I14" s="30"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2575,7 +2578,7 @@
       <c r="I15" s="33"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2583,7 +2586,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2591,7 +2594,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2599,7 +2602,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2607,7 +2610,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2615,7 +2618,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -2623,7 +2626,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2638,7 +2641,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
@@ -2650,7 +2653,7 @@
     <col min="10" max="10" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2666,7 +2669,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2693,7 +2696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2711,7 +2714,7 @@
       </c>
       <c r="J4" s="39"/>
     </row>
-    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2749,7 +2752,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2769,7 +2772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2777,7 +2780,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2785,7 +2788,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2793,7 +2796,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2819,7 +2822,7 @@
       </c>
       <c r="J11" s="28"/>
     </row>
-    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2833,7 +2836,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="31"/>
     </row>
-    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2855,7 +2858,7 @@
       <c r="I13" s="30"/>
       <c r="J13" s="31"/>
     </row>
-    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2869,7 +2872,7 @@
       <c r="I14" s="30"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2891,7 +2894,7 @@
       <c r="I15" s="33"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2899,7 +2902,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2907,7 +2910,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2915,7 +2918,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2923,7 +2926,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2931,7 +2934,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -2939,7 +2942,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2956,7 +2959,7 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
@@ -2968,7 +2971,7 @@
     <col min="10" max="10" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2976,7 +2979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2984,7 +2987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3011,7 +3014,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3031,7 +3034,7 @@
       </c>
       <c r="J4" s="39"/>
     </row>
-    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3050,7 +3053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3069,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3090,7 +3093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3098,7 +3101,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3106,7 +3109,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3114,7 +3117,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3143,7 +3146,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3157,7 +3160,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="31"/>
     </row>
-    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3179,7 +3182,7 @@
       <c r="I13" s="30"/>
       <c r="J13" s="31"/>
     </row>
-    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3193,7 +3196,7 @@
       <c r="I14" s="30"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3215,7 +3218,7 @@
       <c r="I15" s="33"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3223,7 +3226,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3231,7 +3234,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3239,7 +3242,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3247,7 +3250,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3255,7 +3258,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -3263,7 +3266,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3280,7 +3283,7 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
@@ -3292,7 +3295,7 @@
     <col min="10" max="10" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3300,7 +3303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3308,7 +3311,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3335,7 +3338,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3396,7 +3399,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3418,7 +3421,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3426,7 +3429,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3434,7 +3437,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3442,7 +3445,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3471,7 +3474,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3485,7 +3488,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="31"/>
     </row>
-    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3507,7 +3510,7 @@
       <c r="I13" s="30"/>
       <c r="J13" s="31"/>
     </row>
-    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3521,7 +3524,7 @@
       <c r="I14" s="30"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3543,7 +3546,7 @@
       <c r="I15" s="33"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3551,7 +3554,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3559,7 +3562,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3567,7 +3570,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3575,7 +3578,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3583,7 +3586,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -3591,7 +3594,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3602,11 +3605,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0708610E-8457-5F44-B8AF-F77AC55F7F39}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
@@ -3618,7 +3623,7 @@
     <col min="10" max="10" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -3634,7 +3639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -3661,7 +3666,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3684,7 +3689,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3703,7 +3708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3722,7 +3727,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3744,7 +3749,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3752,7 +3757,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3760,7 +3765,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3768,7 +3773,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3792,12 +3797,12 @@
       <c r="I11" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="28" t="e">
-        <f>MODE(Table7[Value])</f>
+      <c r="J11" s="28" t="e" cm="1">
+        <f t="array" ref="J11">_xlfn.MODE.MULT(Table7[Value])</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3809,9 +3814,12 @@
       <c r="F12" s="20"/>
       <c r="H12" s="29"/>
       <c r="I12" s="30"/>
-      <c r="J12" s="31"/>
-    </row>
-    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="28" t="e" cm="1">
+        <f t="array" ref="J12">_xlfn.MODE.MULT(Table7[Value])</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3833,7 +3841,7 @@
       <c r="I13" s="30"/>
       <c r="J13" s="31"/>
     </row>
-    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3847,7 +3855,7 @@
       <c r="I14" s="30"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3869,7 +3877,7 @@
       <c r="I15" s="33"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3877,15 +3885,18 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="4">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3893,7 +3904,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3901,7 +3912,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3909,7 +3920,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -3917,7 +3928,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>